<commit_message>
Change aio courier price
</commit_message>
<xml_diff>
--- a/public/suppliers.xlsx
+++ b/public/suppliers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="aio" sheetId="1" state="visible" r:id="rId3"/>
@@ -54,9 +54,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -150,7 +149,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,7 +314,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>13.01</v>
+        <v>14.63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,7 +346,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>